<commit_message>
adding Method on documents
</commit_message>
<xml_diff>
--- a/documents/PR_TestPlan.xlsx
+++ b/documents/PR_TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mylambton-my.sharepoint.com/personal/c0785370_mylambton_ca/Documents/TERM3/AML3406_CapstoneProject/ProductRecognition_code/testing/Capstone-ProdRecognition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mylambton-my.sharepoint.com/personal/c0785370_mylambton_ca/Documents/TERM3/AML3406_CapstoneProject/ProductRecognition_code/testing/Capstone-ProdRecognition/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD803808-378A-4257-BAC7-DCDA4DAFE2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{BD803808-378A-4257-BAC7-DCDA4DAFE2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47D7877-2E7B-46C5-A9E3-F8691CC0D2C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" activeTab="1" xr2:uid="{55CCEEE6-8650-4C08-B0D9-CE39CD234BC1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{55CCEEE6-8650-4C08-B0D9-CE39CD234BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
   <si>
     <t>Step #</t>
   </si>
@@ -49,12 +49,6 @@
     <t xml:space="preserve">Test data </t>
   </si>
   <si>
-    <t>15 test images</t>
-  </si>
-  <si>
-    <t>15 new images</t>
-  </si>
-  <si>
     <t>Uploaded new photo must be correctly identified.</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>User must be able to access the webpage and click Automotive radio button</t>
   </si>
   <si>
-    <t>User must be able to can upload photo under this section</t>
-  </si>
-  <si>
     <t>Assigned to</t>
   </si>
   <si>
@@ -122,6 +113,30 @@
   </si>
   <si>
     <t>Assigned To</t>
+  </si>
+  <si>
+    <t>10 test images</t>
+  </si>
+  <si>
+    <t>10 new images</t>
+  </si>
+  <si>
+    <t>User must be able to upload photo under this section</t>
+  </si>
+  <si>
+    <t>Angelica</t>
+  </si>
+  <si>
+    <t>Jonatas</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>Akshita</t>
+  </si>
+  <si>
+    <t>Jon/Angelica</t>
   </si>
 </sst>
 </file>
@@ -327,7 +342,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -346,27 +361,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -682,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A33DA54-5109-49CB-AC3E-603E1CCCE6E0}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +688,7 @@
     <col min="4" max="4" width="104.5546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.88671875" style="3"/>
     <col min="10" max="10" width="16" style="3" hidden="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="3"/>
@@ -706,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -718,10 +712,10 @@
         <v>2</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -729,20 +723,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -750,20 +746,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="J4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -771,414 +769,460 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <v>2</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>3</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <v>4</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <v>5</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8">
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="8">
         <v>3</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8">
         <v>4</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="8">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>3</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>4</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>5</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="8">
         <v>1</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="8">
         <v>2</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="8">
         <v>3</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="8">
         <v>4</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="18">
         <v>5</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
@@ -1205,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F991D9-A830-457E-912F-3DE1CAF747D0}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1218,13 +1262,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>